<commit_message>
Update PHPExcel version (commit 6)
</commit_message>
<xml_diff>
--- a/app/vendors/PHPExcel/Tests/01simple.xlsx
+++ b/app/vendors/PHPExcel/Tests/01simple.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+  <si>
+    <t xml:space="preserve">                Hello</t>
+  </si>
   <si>
     <t>Hello</t>
   </si>
@@ -27,13 +30,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <u val="none"/>
       <color rgb="FF000000"/>
     </font>
@@ -53,16 +54,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border outline="true"/>
+    <border/>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="1" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0">
+  <cellXfs count="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -359,7 +357,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <sheetPr codeName="Simple">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
   <dimension ref="A1:D2"/>
@@ -370,7 +368,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.10" customWidth="true"/>
+    <col min="1" max="1" width="9.1" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -378,21 +376,21 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.70" right="0.70" top="0.75" bottom="0.75" header="0.30" footer="0.30"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" fitToHeight="0" fitToWidth="0"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>

</xml_diff>